<commit_message>
Updated Motor IDs file
</commit_message>
<xml_diff>
--- a/Motor IDs.xlsx
+++ b/Motor IDs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gian.l\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gian.l\Documents\Code\2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08C5850D-EA8A-4519-926A-02629D05B109}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C9B1417-C3F7-438D-9125-5E090AB0CD7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6555" xr2:uid="{DEB9AF05-60E4-4891-93B1-26B16F6DCEAC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>front</t>
   </si>
@@ -67,6 +67,42 @@
   </si>
   <si>
     <t>Pick up and Transport</t>
+  </si>
+  <si>
+    <t>Swerve Home</t>
+  </si>
+  <si>
+    <t>Front left</t>
+  </si>
+  <si>
+    <t>Front right</t>
+  </si>
+  <si>
+    <t>Back left</t>
+  </si>
+  <si>
+    <t>Back right</t>
+  </si>
+  <si>
+    <t>Home Relative to Halsensor</t>
+  </si>
+  <si>
+    <t>Halsensor position relative to home</t>
+  </si>
+  <si>
+    <t>Swerve drive PID</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -418,15 +454,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F2AB0B-EC99-471D-9961-BA453810D094}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.9296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.86328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -436,8 +477,17 @@
       <c r="C1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -447,8 +497,18 @@
       <c r="C2">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>-8.9524135589599592</v>
+      </c>
+      <c r="G2">
+        <f>-F2+9</f>
+        <v>17.952413558959961</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -458,8 +518,30 @@
       <c r="C3">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>-8.7857446670532209</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G5" si="0">-F3+9</f>
+        <v>17.785744667053223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>-8.9047937393188406</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>17.904793739318841</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -469,8 +551,18 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5">
+        <v>-8.9524135589599592</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>17.952413558959961</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -481,7 +573,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -492,36 +584,59 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12">
+        <v>1.66E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -529,12 +644,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>9</v>
       </c>

</xml_diff>